<commit_message>
Peri clase del segundo parcial
</commit_message>
<xml_diff>
--- a/Parcial 1/Clases/01 funciones basicas.xlsx
+++ b/Parcial 1/Clases/01 funciones basicas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="1" xr2:uid="{8FD00284-4FBE-4D84-BBA6-DE502194D9FD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="4" xr2:uid="{8FD00284-4FBE-4D84-BBA6-DE502194D9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastos" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
   <si>
     <t>Gastos 2018</t>
   </si>
@@ -440,6 +440,36 @@
   </si>
   <si>
     <t>Funcion</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>=ABS($A$2)</t>
+  </si>
+  <si>
+    <t>=ENTERO($A$3)</t>
+  </si>
+  <si>
+    <t>=FACT.DOBLE($A$4)</t>
+  </si>
+  <si>
+    <t>=MULTIPLO.SUPERIOR($A$5,10)</t>
+  </si>
+  <si>
+    <t>=TRUNCAR($A$6)</t>
+  </si>
+  <si>
+    <t>=TRUNCAR($A$7)</t>
+  </si>
+  <si>
+    <t>=TRUNCAR($A$8)</t>
+  </si>
+  <si>
+    <t>&lt;- Comision</t>
+  </si>
+  <si>
+    <t>TOTAL CON COMISION</t>
   </si>
 </sst>
 </file>
@@ -544,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -584,13 +614,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1190,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF03F8E-6375-45CF-A60D-0F40794D5504}">
   <dimension ref="A2:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A28" sqref="A21:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1206,21 +1239,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="4" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
@@ -2854,13 +2887,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D878C342-2C11-4733-A5B6-99AC33AF7F22}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.86328125" customWidth="1"/>
+    <col min="2" max="2" width="26.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.9296875" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -2873,12 +2906,18 @@
       <c r="B1" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>-23</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="1">
         <f>ABS($A$2)</f>
         <v>23</v>
       </c>
@@ -2887,7 +2926,10 @@
       <c r="A3" s="1">
         <v>6.5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="1">
         <f>INT($A$3)</f>
         <v>6</v>
       </c>
@@ -2896,7 +2938,10 @@
       <c r="A4" s="1">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="1">
         <f>FACTDOUBLE($A$4)</f>
         <v>945</v>
       </c>
@@ -2905,7 +2950,10 @@
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="1">
         <f>CEILING($A$5,10)</f>
         <v>10</v>
       </c>
@@ -2914,7 +2962,10 @@
       <c r="A6" s="1">
         <v>-12.986000000000001</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="1">
         <f>TRUNC($A$6)</f>
         <v>-12</v>
       </c>
@@ -2923,7 +2974,10 @@
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1">
         <f>TRUNC($A$7)</f>
         <v>2</v>
       </c>
@@ -2932,7 +2986,10 @@
       <c r="A8" s="1">
         <v>-33</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="1">
         <f>TRUNC($A$8)</f>
         <v>-33</v>
       </c>
@@ -3090,7 +3147,7 @@
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
@@ -3129,7 +3186,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3213,8 +3270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B755F62B-F1F4-4E4C-8E19-59F3D85CC2A6}">
   <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3826,8 +3883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CBA0946-37D9-4769-8659-CC326920F503}">
   <dimension ref="A2:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="A1:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3840,14 +3897,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
@@ -3863,7 +3920,7 @@
         <v>69</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>83</v>
@@ -4148,6 +4205,9 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>0.1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
       </c>
       <c r="C18" t="s">
         <v>69</v>

</xml_diff>